<commit_message>
Upgrades to config file, remove max labour hard coding
</commit_message>
<xml_diff>
--- a/Jobs.xlsx
+++ b/Jobs.xlsx
@@ -1,49 +1,238 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stuff\isw\code\out2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="RANDBETWEEN">#NAME?</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="152511"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+  <si>
+    <t>Job ID</t>
+  </si>
+  <si>
+    <t>Processing Time(hrs)</t>
+  </si>
+  <si>
+    <t>Due date (hrs)</t>
+  </si>
+  <si>
+    <t>Production Cost (Rs/hr)</t>
+  </si>
+  <si>
+    <t>PenaltCost (Rs/hr)</t>
+  </si>
+  <si>
+    <t>Demand (Quantity/shift)</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>J19</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>J21</t>
+  </si>
+  <si>
+    <t>J22</t>
+  </si>
+  <si>
+    <t>J23</t>
+  </si>
+  <si>
+    <t>J24</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>J29</t>
+  </si>
+  <si>
+    <t>J30</t>
+  </si>
+  <si>
+    <t>J31</t>
+  </si>
+  <si>
+    <t>J32</t>
+  </si>
+  <si>
+    <t>J33</t>
+  </si>
+  <si>
+    <t>J34</t>
+  </si>
+  <si>
+    <t>J35</t>
+  </si>
+  <si>
+    <t>J36</t>
+  </si>
+  <si>
+    <t>J37</t>
+  </si>
+  <si>
+    <t>J38</t>
+  </si>
+  <si>
+    <t>J39</t>
+  </si>
+  <si>
+    <t>J40</t>
+  </si>
+  <si>
+    <t>J41</t>
+  </si>
+  <si>
+    <t>J42</t>
+  </si>
+  <si>
+    <t>J43</t>
+  </si>
+  <si>
+    <t>J44</t>
+  </si>
+  <si>
+    <t>J45</t>
+  </si>
+  <si>
+    <t>J46</t>
+  </si>
+  <si>
+    <t>J47</t>
+  </si>
+  <si>
+    <t>J48</t>
+  </si>
+  <si>
+    <t>J49</t>
+  </si>
+  <si>
+    <t>J50</t>
+  </si>
+  <si>
+    <t>J51</t>
+  </si>
+  <si>
+    <t>J52</t>
+  </si>
+  <si>
+    <t>J53</t>
+  </si>
+  <si>
+    <t>J54</t>
+  </si>
+  <si>
+    <t>J55</t>
+  </si>
+  <si>
+    <t>J56</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <sz val="10"/>
-      <strike val="0"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,89 +245,372 @@
   </fills>
   <borders count="2">
     <border>
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:H57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.142308"/>
-    <col min="2" max="2" style="1" width="17.71" customWidth="1"/>
-    <col min="3" max="3" style="1" width="13.43" customWidth="1"/>
-    <col min="4" max="4" style="1" width="21.14" customWidth="1"/>
-    <col min="5" max="5" style="1" width="16.57" customWidth="1"/>
-    <col min="6" max="6" style="1" width="21" customWidth="1"/>
-    <col min="7" max="8" style="1" width="9.142308"/>
-    <col min="9" max="16384" style="1"/>
+    <col min="1" max="1" width="9.125" style="1"/>
+    <col min="2" max="2" width="17.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9.125" style="1"/>
+    <col min="9" max="16384" width="0" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="str">
-        <v>Job ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Processing Time(hrs)</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Due date (hrs)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Production Cost (Rs/hr)</v>
-      </c>
-      <c r="E1" t="str">
-        <v>PenaltCost (Rs/hr) </v>
-      </c>
-      <c r="F1" t="str">
-        <v>Demand (Quantity/shift)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="str">
-        <v>J1</v>
+    <row r="1" spans="1:7" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.25">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>206</v>
@@ -156,13 +628,13 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="str">
-        <v>J2</v>
+        <f t="shared" ref="G2:G7" ca="1" si="0">RANDBETWEEN(180,220)</f>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>195</v>
@@ -180,13 +652,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="str">
-        <v>J3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25">
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>193</v>
@@ -204,13 +676,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="str">
-        <v>J4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25">
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>203</v>
@@ -228,13 +700,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="str">
-        <v>J5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.25">
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>188</v>
@@ -252,13 +724,13 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="str">
-        <v>J6</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.25">
+      <c r="A7" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>220</v>
@@ -276,13 +748,13 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="str">
-        <v>J7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25">
+      <c r="A8" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>235</v>
@@ -300,13 +772,13 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f>1440-SUM(G2:G7)</f>
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="str">
-        <v>J8</v>
+        <f ca="1">1440-SUM(G2:G7)</f>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.25">
+      <c r="A9" t="s">
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>182</v>
@@ -324,13 +796,13 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="str">
-        <v>J9</v>
+        <f t="shared" ref="G9:G14" ca="1" si="1">RANDBETWEEN(180,220)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.25">
+      <c r="A10" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>189</v>
@@ -348,13 +820,13 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="str">
-        <v>J10</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>181</v>
@@ -372,13 +844,13 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="str">
-        <v>J11</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.25">
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>191</v>
@@ -396,13 +868,13 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="str">
-        <v>J12</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25">
+      <c r="A13" t="s">
+        <v>17</v>
       </c>
       <c r="B13" s="2">
         <v>192</v>
@@ -420,13 +892,13 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="str">
-        <v>J13</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.25">
+      <c r="A14" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>213</v>
@@ -444,13 +916,13 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="str">
-        <v>J14</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.25">
+      <c r="A15" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="2">
         <v>292</v>
@@ -468,13 +940,13 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <f>1440-SUM(G9:G14)</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="str">
-        <v>J15</v>
+        <f ca="1">1440-SUM(G9:G14)</f>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.25">
+      <c r="A16" t="s">
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>182</v>
@@ -492,13 +964,13 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="str">
-        <v>J16</v>
+        <f t="shared" ref="G16:G21" ca="1" si="2">RANDBETWEEN(180,220)</f>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25">
+      <c r="A17" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>205</v>
@@ -516,13 +988,13 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="str">
-        <v>J17</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.25">
+      <c r="A18" t="s">
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>202</v>
@@ -540,13 +1012,13 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="str">
-        <v>J18</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.25">
+      <c r="A19" t="s">
+        <v>23</v>
       </c>
       <c r="B19" s="2">
         <v>188</v>
@@ -564,13 +1036,13 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="str">
-        <v>J19</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.25">
+      <c r="A20" t="s">
+        <v>24</v>
       </c>
       <c r="B20" s="2">
         <v>214</v>
@@ -588,13 +1060,13 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="str">
-        <v>J20</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.25">
+      <c r="A21" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="2">
         <v>207</v>
@@ -612,13 +1084,13 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="str">
-        <v>J21</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.25">
+      <c r="A22" t="s">
+        <v>26</v>
       </c>
       <c r="B22" s="2">
         <v>242</v>
@@ -636,13 +1108,13 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <f>1440-SUM(G16:G21)</f>
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="str">
-        <v>J22</v>
+        <f ca="1">1440-SUM(G16:G21)</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.25">
+      <c r="A23" t="s">
+        <v>27</v>
       </c>
       <c r="B23">
         <v>198</v>
@@ -660,13 +1132,13 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="str">
-        <v>J23</v>
+        <f t="shared" ref="G23:G28" ca="1" si="3">RANDBETWEEN(180,220)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.25">
+      <c r="A24" t="s">
+        <v>28</v>
       </c>
       <c r="B24">
         <v>181</v>
@@ -684,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="str">
-        <v>J24</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.25">
+      <c r="A25" t="s">
+        <v>29</v>
       </c>
       <c r="B25">
         <v>196</v>
@@ -708,13 +1180,13 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="str">
-        <v>J25</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.25">
+      <c r="A26" t="s">
+        <v>30</v>
       </c>
       <c r="B26">
         <v>203</v>
@@ -732,13 +1204,13 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="str">
-        <v>J26</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.25">
+      <c r="A27" t="s">
+        <v>31</v>
       </c>
       <c r="B27">
         <v>183</v>
@@ -756,13 +1228,13 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="str">
-        <v>J27</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.25">
+      <c r="A28" t="s">
+        <v>32</v>
       </c>
       <c r="B28">
         <v>193</v>
@@ -780,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>193</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="str">
-        <v>J28</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.25">
+      <c r="A29" t="s">
+        <v>33</v>
       </c>
       <c r="B29">
         <v>286</v>
@@ -804,13 +1276,13 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <f>1440-SUM(G23:G28)</f>
-        <v>286</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="str">
-        <v>J29</v>
+        <f ca="1">1440-SUM(G23:G28)</f>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14.25">
+      <c r="A30" t="s">
+        <v>34</v>
       </c>
       <c r="B30">
         <v>191</v>
@@ -828,13 +1300,13 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="str">
-        <v>J30</v>
+        <f t="shared" ref="G30:G35" ca="1" si="4">RANDBETWEEN(180,220)</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.25">
+      <c r="A31" t="s">
+        <v>35</v>
       </c>
       <c r="B31">
         <v>192</v>
@@ -852,13 +1324,13 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="str">
-        <v>J31</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14.25">
+      <c r="A32" t="s">
+        <v>36</v>
       </c>
       <c r="B32">
         <v>190</v>
@@ -876,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="str">
-        <v>J32</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14.25">
+      <c r="A33" t="s">
+        <v>37</v>
       </c>
       <c r="B33">
         <v>182</v>
@@ -900,13 +1372,13 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="str">
-        <v>J33</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="14.25">
+      <c r="A34" t="s">
+        <v>38</v>
       </c>
       <c r="B34">
         <v>196</v>
@@ -924,13 +1396,13 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="str">
-        <v>J34</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.25">
+      <c r="A35" t="s">
+        <v>39</v>
       </c>
       <c r="B35">
         <v>184</v>
@@ -948,13 +1420,13 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="str">
-        <v>J35</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="14.25">
+      <c r="A36" t="s">
+        <v>40</v>
       </c>
       <c r="B36">
         <v>305</v>
@@ -972,13 +1444,13 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <f>1440-SUM(G30:G35)</f>
-        <v>305</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="str">
-        <v>J36</v>
+        <f ca="1">1440-SUM(G30:G35)</f>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="14.25">
+      <c r="A37" t="s">
+        <v>41</v>
       </c>
       <c r="B37">
         <v>190</v>
@@ -996,13 +1468,13 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="str">
-        <v>J37</v>
+        <f t="shared" ref="G37:G42" ca="1" si="5">RANDBETWEEN(180,220)</f>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14.25">
+      <c r="A38" t="s">
+        <v>42</v>
       </c>
       <c r="B38">
         <v>219</v>
@@ -1020,13 +1492,13 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="str">
-        <v>J38</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="14.25">
+      <c r="A39" t="s">
+        <v>43</v>
       </c>
       <c r="B39">
         <v>218</v>
@@ -1044,13 +1516,13 @@
         <v>1</v>
       </c>
       <c r="G39">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>188</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" t="str">
-        <v>J39</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="14.25">
+      <c r="A40" t="s">
+        <v>44</v>
       </c>
       <c r="B40">
         <v>182</v>
@@ -1068,13 +1540,13 @@
         <v>1</v>
       </c>
       <c r="G40">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="str">
-        <v>J40</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="14.25">
+      <c r="A41" t="s">
+        <v>45</v>
       </c>
       <c r="B41">
         <v>193</v>
@@ -1092,13 +1564,13 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" t="str">
-        <v>J41</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="14.25">
+      <c r="A42" t="s">
+        <v>46</v>
       </c>
       <c r="B42">
         <v>186</v>
@@ -1116,13 +1588,13 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>219</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" t="str">
-        <v>J42</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="14.25">
+      <c r="A43" t="s">
+        <v>47</v>
       </c>
       <c r="B43">
         <v>252</v>
@@ -1140,13 +1612,13 @@
         <v>1</v>
       </c>
       <c r="G43">
-        <f>1440-SUM(G37:G42)</f>
-        <v>227</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="str">
-        <v>J43</v>
+        <f ca="1">1440-SUM(G37:G42)</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="14.25">
+      <c r="A44" t="s">
+        <v>48</v>
       </c>
       <c r="B44">
         <v>216</v>
@@ -1164,13 +1636,13 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>216</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="str">
-        <v>J44</v>
+        <f t="shared" ref="G44:G49" ca="1" si="6">RANDBETWEEN(180,220)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="14.25">
+      <c r="A45" t="s">
+        <v>49</v>
       </c>
       <c r="B45">
         <v>195</v>
@@ -1188,13 +1660,13 @@
         <v>1</v>
       </c>
       <c r="G45">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="str">
-        <v>J45</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="14.25">
+      <c r="A46" t="s">
+        <v>50</v>
       </c>
       <c r="B46">
         <v>196</v>
@@ -1212,13 +1684,13 @@
         <v>1</v>
       </c>
       <c r="G46">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>196</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="str">
-        <v>J46</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="14.25">
+      <c r="A47" t="s">
+        <v>51</v>
       </c>
       <c r="B47">
         <v>216</v>
@@ -1236,13 +1708,13 @@
         <v>1</v>
       </c>
       <c r="G47">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>216</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="str">
-        <v>J47</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="14.25">
+      <c r="A48" t="s">
+        <v>52</v>
       </c>
       <c r="B48">
         <v>187</v>
@@ -1260,13 +1732,13 @@
         <v>1</v>
       </c>
       <c r="G48">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" t="str">
-        <v>J48</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="14.25">
+      <c r="A49" t="s">
+        <v>53</v>
       </c>
       <c r="B49">
         <v>197</v>
@@ -1284,13 +1756,13 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" t="str">
-        <v>J49</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="14.25">
+      <c r="A50" t="s">
+        <v>54</v>
       </c>
       <c r="B50">
         <v>233</v>
@@ -1308,13 +1780,13 @@
         <v>1</v>
       </c>
       <c r="G50">
-        <f>1440-SUM(G44:G49)</f>
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="str">
-        <v>J50</v>
+        <f ca="1">1440-SUM(G44:G49)</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="14.25">
+      <c r="A51" t="s">
+        <v>55</v>
       </c>
       <c r="B51">
         <v>218</v>
@@ -1332,13 +1804,13 @@
         <v>1</v>
       </c>
       <c r="G51">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" t="str">
-        <v>J51</v>
+        <f t="shared" ref="G51:G56" ca="1" si="7">RANDBETWEEN(180,220)</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="14.25">
+      <c r="A52" t="s">
+        <v>56</v>
       </c>
       <c r="B52">
         <v>181</v>
@@ -1356,13 +1828,13 @@
         <v>1</v>
       </c>
       <c r="G52">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" t="str">
-        <v>J52</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="14.25">
+      <c r="A53" t="s">
+        <v>57</v>
       </c>
       <c r="B53">
         <v>204</v>
@@ -1380,13 +1852,13 @@
         <v>1</v>
       </c>
       <c r="G53">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="str">
-        <v>J53</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="14.25">
+      <c r="A54" t="s">
+        <v>58</v>
       </c>
       <c r="B54">
         <v>212</v>
@@ -1404,13 +1876,13 @@
         <v>1</v>
       </c>
       <c r="G54">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>212</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" t="str">
-        <v>J54</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="14.25">
+      <c r="A55" t="s">
+        <v>59</v>
       </c>
       <c r="B55">
         <v>182</v>
@@ -1428,13 +1900,13 @@
         <v>1</v>
       </c>
       <c r="G55">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" t="str">
-        <v>J55</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="14.25">
+      <c r="A56" t="s">
+        <v>60</v>
       </c>
       <c r="B56">
         <v>207</v>
@@ -1452,13 +1924,13 @@
         <v>1</v>
       </c>
       <c r="G56">
-        <f>RANDBETWEEN(180,220)</f>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="str">
-        <v>J56</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="14.25">
+      <c r="A57" t="s">
+        <v>61</v>
       </c>
       <c r="B57">
         <v>236</v>
@@ -1476,14 +1948,13 @@
         <v>1</v>
       </c>
       <c r="G57">
-        <f>1440-SUM(G51:G56)</f>
-        <v>236</v>
+        <f ca="1">1440-SUM(G51:G56)</f>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
</xml_diff>